<commit_message>
OSM export done for single data and single has-a relationship
</commit_message>
<xml_diff>
--- a/employee.xlsx
+++ b/employee.xlsx
@@ -6,13 +6,32 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="employee" r:id="rId3" sheetId="1"/>
+    <sheet name="address" r:id="rId3" sheetId="1"/>
+    <sheet name="employee" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>house</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Forest Lodge</t>
+  </si>
+  <si>
+    <t>S.S. Academy Road</t>
+  </si>
   <si>
     <t>name</t>
   </si>
@@ -23,13 +42,13 @@
     <t>address_id</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>Mainul</t>
   </si>
   <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>25</t>
   </si>
 </sst>
 </file>
@@ -105,4 +124,45 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactoring - One to One relationship, tested with multiple data set. Handled duplicate data insertion into sheet.
</commit_message>
<xml_diff>
--- a/employee.xlsx
+++ b/employee.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -42,13 +42,34 @@
     <t>address_id</t>
   </si>
   <si>
-    <t/>
+    <t>1</t>
   </si>
   <si>
     <t>Mainul</t>
   </si>
   <si>
     <t>25</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Avijan 9/2</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Hasan</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>Siam</t>
+  </si>
+  <si>
+    <t>16</t>
   </si>
 </sst>
 </file>
@@ -93,7 +114,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -121,6 +142,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -128,7 +160,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -162,6 +194,34 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>